<commit_message>
table1 to pdf. not able to do footnotes
</commit_message>
<xml_diff>
--- a/tables/table1.xlsx
+++ b/tables/table1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="156">
   <si>
     <t xml:space="preserve">Taxonomy</t>
   </si>
@@ -114,25 +114,7 @@
     <t xml:space="preserve">Greed Avoidance</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Social Dominance Orientation </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Leone, L., 2012)</t>
-    </r>
+    <t xml:space="preserve">- Social Dominance Orientation (Leone, L., 2012)</t>
   </si>
   <si>
     <t xml:space="preserve">Modesty</t>
@@ -164,24 +146,16 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- Callous affect (Gaughan et al., 2012); + Diversity</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+      <t xml:space="preserve">- Callous affect (Gaughan et al., 2012); + Diversity </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -191,6 +165,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">McAbee, Oswald, Connelly, 2014</t>
     </r>
@@ -201,6 +176,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -221,6 +197,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+ Emision-reduction behavior (Brick &amp; Lewis, 2014) + Leadership </t>
     </r>
@@ -231,6 +208,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -240,6 +218,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">McAbee et al. 2014</t>
     </r>
@@ -250,6 +229,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -382,6 +362,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+ Emision-reduction behavior </t>
     </r>
@@ -392,6 +373,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -401,6 +383,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Brick &amp; Lewis, 2014</t>
     </r>
@@ -411,6 +394,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -516,25 +500,7 @@
     <t xml:space="preserve">Aesthetic</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Right Wing Authoritarism </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Leone, L., 2012); + Emision-reduction behavior (Brick &amp; Lewis, 2014) + Artistic appreciation (McAbee et al, 2014)</t>
-    </r>
+    <t xml:space="preserve">- Right Wing Authoritarism (Leone, L., 2012); + Emision-reduction behavior (Brick &amp; Lewis, 2014) + Artistic appreciation (McAbee et al, 2014)</t>
   </si>
   <si>
     <t xml:space="preserve">Unconventionality</t>
@@ -546,6 +512,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Political Conservatism </t>
     </r>
@@ -556,6 +523,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -565,6 +533,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Brick &amp; Lewis, 2014</t>
     </r>
@@ -575,6 +544,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -607,25 +577,7 @@
     <t xml:space="preserve">Depression</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Attachment Anxiety (Noftle &amp; Shaver, 2006); +</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Alexithymia (Bagby et al. 1993) - Satisfaction with life (Schimmack et al., 2004)</t>
-    </r>
+    <t xml:space="preserve">+ Attachment Anxiety (Noftle &amp; Shaver, 2006); + Alexithymia (Bagby et al. 1993) - Satisfaction with life (Schimmack et al., 2004)</t>
   </si>
   <si>
     <t xml:space="preserve">Self-Consciousness</t>
@@ -834,24 +786,16 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- Interpersonal manipulation (Gaughan, 2014); -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Supervisor rating </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+      <t xml:space="preserve">- Interpersonal manipulation (Gaughan, 2014); - Supervisor rating </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -861,6 +805,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Piedmont &amp; Weinstein, 1994</t>
     </r>
@@ -871,6 +816,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -999,24 +945,16 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- Attachment anxiety (Noftle &amp; Shaver, 2006); - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Dysregulation / Disinhibition </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+      <t xml:space="preserve">- Attachment anxiety (Noftle &amp; Shaver, 2006); - Dysregulation / Disinhibition </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -1026,6 +964,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Gaughan et. al, 2009</t>
     </r>
@@ -1036,6 +975,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -1044,25 +984,7 @@
     <t xml:space="preserve">Deliberation</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Erratic life-style (Gaughan, 2014); -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Alcohol related problems (Ruiz et al., 2010)</t>
-    </r>
+    <t xml:space="preserve">- Erratic life-style (Gaughan, 2014); - Alcohol related problems (Ruiz et al., 2010)</t>
   </si>
   <si>
     <t xml:space="preserve">BFI-2</t>
@@ -1071,33 +993,277 @@
     <t xml:space="preserve">*</t>
   </si>
   <si>
+    <t xml:space="preserve">- Conformity, - Tradition, + Stimulation, + Positive affect (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Power </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Soto &amp; John, 2016</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Energy level</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Purpose in life, + Self-acceptance, + Social connectedness (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Compassion</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Benevolence, - Power, + Positive relations (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Respectfulness</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Conformity </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Soto &amp; John, 2016</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Universalism, + Likability (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Security </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Soto &amp; John, 2016</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Productiveness</t>
   </si>
   <si>
+    <t xml:space="preserve">- Hedonism, + Achievement, + Environmental mastery (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Responsability</t>
   </si>
   <si>
+    <t xml:space="preserve">- Stimulation, + Autonomy (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Negative Emotionality</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Autonomy </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Soto &amp; John, 2016</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- Positive relations, - Purpose in life, - Environmental mastery, -Self-acceptance, - Positive affect (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emotional Volatility</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Stress resistance </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Soto &amp; John, 2016</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Open-mindedness</t>
   </si>
   <si>
     <t xml:space="preserve">Intellectual curiosity</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Self-direction, + Personal growth (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aesthetic Sensitivity</t>
   </si>
   <si>
@@ -1110,18 +1276,112 @@
     <t xml:space="preserve">Anger</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Academic achievement school </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rosander &amp; Bäckstörm, 2014</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Inmoderation</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Hangover symptoms </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McAdams &amp; Donnellan, 2009</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Friendliness</t>
   </si>
   <si>
     <t xml:space="preserve">Activity Level</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Alcohol Use, + Drinking problems (McAdams &amp; Donnellan, 2009)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cheerfulness</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Addictive mobile phone usage style (Siddiqui, 2011)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Openness to Experience</t>
   </si>
   <si>
@@ -1140,9 +1400,15 @@
     <t xml:space="preserve">Liberalism</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Trendy mobile phone usage style (Siddiqui, 2011)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Morality</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Thrifty mobile phone usage style (Siddiqui, 2011)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cooperation</t>
   </si>
   <si>
@@ -1156,6 +1422,94 @@
   </si>
   <si>
     <t xml:space="preserve">Achievement-striving</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Academic Performance </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rosander, Bäckström &amp; Sternberg, 2011</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ General health behaviors </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Hagger-Johnson &amp; Whiteman, 2007</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Cautiousness</t>
@@ -1168,7 +1522,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1204,19 +1558,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1275,7 +1616,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1312,14 +1653,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1347,8 +1680,8 @@
   </sheetPr>
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1414,9 +1747,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4" t="n">
-        <v>0.82</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1493,9 +1824,7 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4" t="n">
-        <v>0.84</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="5"/>
       <c r="G9" s="4"/>
     </row>
@@ -1560,9 +1889,7 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4" t="n">
-        <v>0.85</v>
-      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="5"/>
       <c r="G14" s="4"/>
     </row>
@@ -1589,7 +1916,7 @@
       <c r="E16" s="4" t="n">
         <v>0.76</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="5" t="s">
         <v>29</v>
       </c>
       <c r="G16" s="4"/>
@@ -1629,9 +1956,7 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4" t="n">
-        <v>0.84</v>
-      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="G19" s="4"/>
     </row>
@@ -1694,9 +2019,7 @@
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="4" t="n">
-        <v>0.84</v>
-      </c>
+      <c r="E24" s="4"/>
       <c r="F24" s="5"/>
       <c r="G24" s="4"/>
     </row>
@@ -1738,7 +2061,7 @@
       <c r="E27" s="4" t="n">
         <v>0.69</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G27" s="4"/>
@@ -1765,9 +2088,7 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="4" t="n">
-        <v>0.81</v>
-      </c>
+      <c r="E29" s="4"/>
       <c r="F29" s="5" t="s">
         <v>47</v>
       </c>
@@ -1800,7 +2121,7 @@
       <c r="E31" s="4" t="n">
         <v>0.52</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="8" t="s">
         <v>52</v>
       </c>
       <c r="G31" s="4"/>
@@ -1864,9 +2185,7 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="4" t="n">
-        <v>0.92</v>
-      </c>
+      <c r="E36" s="4"/>
       <c r="F36" s="5"/>
       <c r="G36" s="4"/>
     </row>
@@ -1880,7 +2199,7 @@
       <c r="E37" s="4" t="n">
         <v>0.78</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G37" s="4"/>
@@ -1965,9 +2284,7 @@
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="4" t="n">
-        <v>0.89</v>
-      </c>
+      <c r="E43" s="4"/>
       <c r="F43" s="5"/>
       <c r="G43" s="4"/>
     </row>
@@ -1996,7 +2313,7 @@
       <c r="E45" s="4" t="n">
         <v>0.72</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="5" t="s">
         <v>71</v>
       </c>
       <c r="G45" s="4"/>
@@ -2052,7 +2369,7 @@
       <c r="E49" s="4" t="n">
         <v>0.73</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="5" t="s">
         <v>77</v>
       </c>
       <c r="G49" s="4"/>
@@ -2064,9 +2381,7 @@
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="4" t="n">
-        <v>0.87</v>
-      </c>
+      <c r="E50" s="4"/>
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
     </row>
@@ -2159,9 +2474,7 @@
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="4" t="n">
-        <v>0.86</v>
-      </c>
+      <c r="E57" s="4"/>
       <c r="F57" s="5"/>
       <c r="G57" s="4"/>
     </row>
@@ -2256,9 +2569,7 @@
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
-      <c r="E64" s="4" t="n">
-        <v>0.9</v>
-      </c>
+      <c r="E64" s="4"/>
       <c r="F64" s="5"/>
       <c r="G64" s="4"/>
     </row>
@@ -2391,7 +2702,9 @@
       <c r="E74" s="4" t="n">
         <v>0.83</v>
       </c>
-      <c r="F74" s="5"/>
+      <c r="F74" s="5" t="s">
+        <v>105</v>
+      </c>
       <c r="G74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,7 +2717,9 @@
       <c r="E75" s="4" t="n">
         <v>0.8</v>
       </c>
-      <c r="F75" s="5"/>
+      <c r="F75" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="G75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,12 +2727,14 @@
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E76" s="4" t="n">
         <v>0.74</v>
       </c>
-      <c r="F76" s="5"/>
+      <c r="F76" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="G76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,12 +2753,14 @@
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E78" s="4" t="n">
         <v>0.68</v>
       </c>
-      <c r="F78" s="5"/>
+      <c r="F78" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="G78" s="4"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2449,12 +2768,14 @@
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E79" s="4" t="n">
         <v>0.66</v>
       </c>
-      <c r="F79" s="5"/>
+      <c r="F79" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="G79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2467,7 +2788,9 @@
       <c r="E80" s="4" t="n">
         <v>0.75</v>
       </c>
-      <c r="F80" s="5"/>
+      <c r="F80" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="G80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2491,7 +2814,9 @@
       <c r="E82" s="4" t="n">
         <v>0.76</v>
       </c>
-      <c r="F82" s="5"/>
+      <c r="F82" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="G82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,12 +2824,14 @@
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E83" s="4" t="n">
         <v>0.74</v>
       </c>
-      <c r="F83" s="5"/>
+      <c r="F83" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="G83" s="4"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,18 +2839,20 @@
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E84" s="4" t="n">
         <v>0.68</v>
       </c>
-      <c r="F84" s="5"/>
+      <c r="F84" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="G84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4"/>
       <c r="B85" s="4" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -2541,7 +2870,9 @@
       <c r="E86" s="4" t="n">
         <v>0.79</v>
       </c>
-      <c r="F86" s="5"/>
+      <c r="F86" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="G86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,7 +2885,9 @@
       <c r="E87" s="4" t="n">
         <v>0.74</v>
       </c>
-      <c r="F87" s="5"/>
+      <c r="F87" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="G87" s="4"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2562,18 +2895,20 @@
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E88" s="4" t="n">
         <v>0.7</v>
       </c>
-      <c r="F88" s="5"/>
+      <c r="F88" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="G88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4"/>
       <c r="B89" s="4" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -2586,12 +2921,14 @@
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E90" s="4" t="n">
         <v>0.78</v>
       </c>
-      <c r="F90" s="5"/>
+      <c r="F90" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="G90" s="4"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,7 +2936,7 @@
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="E91" s="4" t="n">
         <v>0.67</v>
@@ -2612,7 +2949,7 @@
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="E92" s="4" t="n">
         <v>0.67</v>
@@ -2631,7 +2968,7 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -2671,7 +3008,7 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="E97" s="4" t="n">
         <v>0.87</v>
@@ -2702,7 +3039,9 @@
       <c r="E99" s="4" t="n">
         <v>0.74</v>
       </c>
-      <c r="F99" s="5"/>
+      <c r="F99" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="G99" s="4"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2710,12 +3049,14 @@
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E100" s="4" t="n">
         <v>0.72</v>
       </c>
-      <c r="F100" s="5"/>
+      <c r="F100" s="5" t="s">
+        <v>133</v>
+      </c>
       <c r="G100" s="4"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,7 +3088,7 @@
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="E103" s="4" t="n">
         <v>0.81</v>
@@ -2786,7 +3127,7 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="E106" s="4" t="n">
         <v>0.71</v>
@@ -2804,7 +3145,9 @@
       <c r="E107" s="4" t="n">
         <v>0.77</v>
       </c>
-      <c r="F107" s="5"/>
+      <c r="F107" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="G107" s="4"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2812,18 +3155,20 @@
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="E108" s="4" t="n">
         <v>0.8</v>
       </c>
-      <c r="F108" s="5"/>
+      <c r="F108" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="G108" s="4"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -2836,7 +3181,7 @@
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="E110" s="4" t="n">
         <v>0.83</v>
@@ -2849,7 +3194,7 @@
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="E111" s="4" t="n">
         <v>0.76</v>
@@ -2875,7 +3220,7 @@
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="E113" s="4" t="n">
         <v>0.72</v>
@@ -2888,7 +3233,7 @@
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="E114" s="4" t="n">
         <v>0.75</v>
@@ -2901,12 +3246,14 @@
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="E115" s="4" t="n">
         <v>0.64</v>
       </c>
-      <c r="F115" s="5"/>
+      <c r="F115" s="5" t="s">
+        <v>145</v>
+      </c>
       <c r="G115" s="4"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,12 +3285,14 @@
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="E118" s="4" t="n">
         <v>0.76</v>
       </c>
-      <c r="F118" s="5"/>
+      <c r="F118" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="G118" s="4"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,7 +3313,7 @@
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="E120" s="4" t="n">
         <v>0.73</v>
@@ -2990,7 +3339,7 @@
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="E122" s="4" t="n">
         <v>0.72</v>
@@ -3014,7 +3363,7 @@
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="E124" s="4" t="n">
         <v>0.63</v>
@@ -3027,7 +3376,7 @@
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="E125" s="4" t="n">
         <v>0.83</v>
@@ -3053,12 +3402,14 @@
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="E127" s="4" t="n">
         <v>0.8</v>
       </c>
-      <c r="F127" s="5"/>
+      <c r="F127" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="G127" s="4"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3071,21 +3422,23 @@
       <c r="E128" s="4" t="n">
         <v>0.73</v>
       </c>
-      <c r="F128" s="5"/>
+      <c r="F128" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="G128" s="4"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="11"/>
-      <c r="B129" s="11"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E129" s="11" t="n">
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E129" s="9" t="n">
         <v>0.87</v>
       </c>
-      <c r="F129" s="12"/>
-      <c r="G129" s="11"/>
+      <c r="F129" s="10"/>
+      <c r="G129" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
finished table1 added references to draft
</commit_message>
<xml_diff>
--- a/tables/table1.xlsx
+++ b/tables/table1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="158">
   <si>
     <t xml:space="preserve">Taxonomy</t>
   </si>
@@ -43,39 +43,63 @@
     <t xml:space="preserve">No. of items</t>
   </si>
   <si>
-    <t xml:space="preserve">HEXACO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200,100,60</t>
+    <t xml:space="preserve">HEXACO-PI-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Lee &amp; Ashton, 2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100*, 60</t>
   </si>
   <si>
     <t xml:space="preserve">Humility</t>
   </si>
   <si>
-    <t xml:space="preserve">- Creativity (Silvia, P., 2011)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Honesty</t>
   </si>
   <si>
     <t xml:space="preserve">Sincerity</t>
   </si>
   <si>
-    <t xml:space="preserve">+ Emision-reduction behavior (Brick &amp; Lewis, 2014)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fairness</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Psychopathy </t>
+    <t xml:space="preserve">- Psychopathy (-.66), - Antisocial behavior (-.44) (Gaughan, Miller, Lynam, 2012); + Ethics/Integrity (.22) (McAbee et al., 2014)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greed Avoidance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Social Dominance Orientation (-.45) (Leone, Chirumbolo, Desimoni, 2012)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modesty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emotionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fearfulness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anxiety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentimentality</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Callous affect (-.68) (Gaughan et al., 2012); + Diversity </t>
     </r>
     <r>
       <rPr>
@@ -96,7 +120,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Gaughan, Miller, Lynam, 2012</t>
+      <t xml:space="preserve">.22</t>
     </r>
     <r>
       <rPr>
@@ -109,53 +133,40 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Greed Avoidance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Social Dominance Orientation (Leone, L., 2012)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modesty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Political Conservatism; + Connectedness to nature (Brick &amp; Lewis, 2014)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emotionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fearfulness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anxiety</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dependence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sentimentality</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Callous affect (Gaughan et al., 2012); + Diversity </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (McAbee, Oswald, Connelly, 2014)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Extraversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Self-Esteem</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Adaptability / Life skills (.25) </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -165,41 +176,42 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">McAbee, Oswald, Connelly, 2014</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McAbee et al., 2014</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Extraversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Self-Esteem</t>
-  </si>
-  <si>
     <t xml:space="preserve">Social Boldness</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Emision-reduction behavior (Brick &amp; Lewis, 2014) + Leadership </t>
+    <t xml:space="preserve">+ Emision-reduction behavior (Brick &amp; Lewis, 2014) + Leadership (.36) (McAbee et al., 2014)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sociability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liveliness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Adaptability / Life skills (.25), + Social responsability (.22), + Health </t>
     </r>
     <r>
       <rPr>
@@ -220,7 +232,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">McAbee et al. 2014</t>
+      <t xml:space="preserve">.21</t>
     </r>
     <r>
       <rPr>
@@ -233,23 +245,51 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Sociability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liveliness</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Adaptability / Life skills </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (McAbee et al., 2014)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Agreeableness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forgivingness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gentleness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flexibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conscientiousness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diligence</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ GPA (.31), + Adaptability / Life skills (.37), + Perseverance </t>
     </r>
     <r>
       <rPr>
@@ -270,7 +310,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">McAbee et al., 2014</t>
+      <t xml:space="preserve">.50</t>
     </r>
     <r>
       <rPr>
@@ -283,41 +323,30 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Agreeableness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forgivingness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gentleness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flexibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patience</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conscientiousness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diligence</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ GPA </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (McAbee et al., 2014)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfectionism</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Emision-reduction behavior </t>
     </r>
     <r>
       <rPr>
@@ -338,7 +367,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">McAbee, 2014</t>
+      <t xml:space="preserve">.25</t>
     </r>
     <r>
       <rPr>
@@ -351,20 +380,30 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Perfectionism</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Emision-reduction behavior </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Brick &amp; Lewis, 2014)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Prudence</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Erratic life-style </t>
     </r>
     <r>
       <rPr>
@@ -385,7 +424,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Brick &amp; Lewis, 2014</t>
+      <t xml:space="preserve">-.58</t>
     </r>
     <r>
       <rPr>
@@ -398,20 +437,108 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Prudence</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Erratic life-style </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Gaughan et al., 2012)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Openness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiential O.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aesthetic</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Emision-reduction behavior (.33) , </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Connectedness to nature (.51)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Brick &amp; Lewis, 2014); </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Right Wing Authoritarism (-.37) (Leone et al., 2012);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Continuous learning (.30) (McAbee, 2014) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Artistic appreciation (.43) (McAbee et al, 2014)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Unconventionality</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Political Conservatism </t>
     </r>
     <r>
       <rPr>
@@ -432,7 +559,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Gaughan et al., 2012</t>
+      <t xml:space="preserve">.29</t>
     </r>
     <r>
       <rPr>
@@ -445,29 +572,44 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Openness</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Creativity (Silvia, p., 2011); + Continuous learning </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Brick &amp; Lewis, 2014)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognitive O.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creativity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inquisitiveness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Continuous learning (.30) </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -477,44 +619,114 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">McAbee, 2014</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">McAbee et al, 2014</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Experiential O.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aesthetic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Right Wing Authoritarism (Leone, L., 2012); + Emision-reduction behavior (Brick &amp; Lewis, 2014) + Artistic appreciation (McAbee et al, 2014)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unconventionality</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Political Conservatism </t>
+    <t xml:space="preserve">NEO-PI-r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(McCrae et al., 2011)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neuroticism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Fearless dominance (-.49) (Gaughan et al, 2009)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angry Hostility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Callous / Manipulation (.29) &amp; Dysregulation / Disinhibition (.48) &amp; Anti social behavior (.26) (Gaughan et al, 2009)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depression</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Attachment Anxiety (.49), + Attachment avoidance (.26) (Noftle &amp; Shaver, 2006); + Alexithymia (.36) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Bagby, Taylor, Parker; 1994); - Satisfaction with life (-.52) (Schimmack et al., 2004); + Avoidant attachment style (.32), + Anxious attachment style (.32) , - Secure attachment style (-.39) (Shaver &amp; Brennan, 1992)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Self-Consciousness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Autism-spectrum Quotient (.33) (Wakabayashi, Baron-Cohen, Wheelwright, 2006); + Avoidant attachment style (.32) (Shaver &amp; Brennan, 1992)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulsiveness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Alcohol related problems (.29) (Ruiz, Pincus &amp; Dickinson, 2010)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vulnerability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warmth</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Secure attachment style (Shaver &amp; Brennan, 1992); -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Attachment avoidance (-.26) (Noftle &amp; Shaver, 2006)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Gregariousness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Autism-spectrum Quotient (-.43) </t>
     </r>
     <r>
       <rPr>
@@ -535,7 +747,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Brick &amp; Lewis, 2014</t>
+      <t xml:space="preserve">Wakabayashi et al., 2006</t>
     </r>
     <r>
       <rPr>
@@ -550,48 +762,24 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Cognitive O.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creativity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inquisitiveness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEO-PI-r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neuroticism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Fearless dominance (Gaughan et al, 2009)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angry Hostility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Callous / Manipulation &amp; Dysregulation / Disinhibition &amp; Anti social behavior (Gaughan et. al, 2009)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Attachment Anxiety (Noftle &amp; Shaver, 2006); + Alexithymia (Bagby et al. 1993) - Satisfaction with life (Schimmack et al., 2004)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Self-Consciousness</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Autism-spectrum Quotient (Wakabayashi et al., 2006) + Avoidant attachment style </t>
+    <t xml:space="preserve">Assertiveness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excitement Seeking</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Fearless dominance </t>
     </r>
     <r>
       <rPr>
@@ -612,7 +800,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Shaver &amp; Brennan, 1992</t>
+      <t xml:space="preserve">.53</t>
     </r>
     <r>
       <rPr>
@@ -625,29 +813,72 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Impulsiveness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Alcohol related problems (Ruiz, Pincus &amp; Dickinson, 2010)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vulnerability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warmth</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Secure attachment style </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Gaughan et al, 2009)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive Emotions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Satisfaction with life (.40) (Schimmack et al., 2004); -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Avoidant attachment style (-.30) (Shaver &amp; Brennan, 1992)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Fantasy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aesthetics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feelings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Alexithymia (-.55) (Bagby et al., 1994)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ SAT verbal (.26) </t>
     </r>
     <r>
       <rPr>
@@ -668,7 +899,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Shaver &amp; Brennan, 1992</t>
+      <t xml:space="preserve">Noftle &amp; Robins, 2007</t>
     </r>
     <r>
       <rPr>
@@ -683,60 +914,85 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Gregariousness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Autism-spectrum Quotient (Wakabayashi et al., 2006)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assertiveness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excitement Seeking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Fearless dominance (Gaughan et al, 2009)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive Emotions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Satisfaction with life (Schimmack et al., 2004)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fantasy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aesthetics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feelings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Alexithymia (Bagby, Taylor, Parker; 1993)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ideas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Values</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ SAT verbal </t>
+    <t xml:space="preserve">Trust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Attachment avoidance (-.26) (Noftle &amp; Shaver, 2006)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Straightforwardness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Interpersonal manipulation (-.75) (Gaughan et al., 2012); - Supervisor rating (Piedmont &amp; Weinstein, 1994); </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Fearless dominance (-.49), - Dysregulation / Disinhibition (-.49) (Gaughan et al, 2009)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Altruism</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Callous affect (-.63), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Antisocial behavior (-.37) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Gaughan et al., 2009);  - Antisocial behavior (-.26)(Gaughan, et al., 2012)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Compliance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tender-Mindedness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Callous affect </t>
     </r>
     <r>
       <rPr>
@@ -757,7 +1013,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Noftle &amp; Robins, 2007</t>
+      <t xml:space="preserve">-.56</t>
     </r>
     <r>
       <rPr>
@@ -770,32 +1026,43 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Trust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Straightforwardness</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Interpersonal manipulation (Gaughan, 2014); - Supervisor rating </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Gaughan et al., 2012)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Competence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutifulness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Dysregulation / Disinhibition (-.49) </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -805,35 +1072,54 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Piedmont &amp; Weinstein, 1994</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gaughan et al, 2009</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Altruism</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Callous affect &amp; antisocial behavior (Gaughan, 2014); - Antisocial behavior </t>
+    <t xml:space="preserve">Achievement Striving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Supervisor rating (.23) (Piedmont &amp; Weinstein, 1994)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self-Discipline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Attachment anxiety (-.35) (Noftle &amp; Shaver, 2006); - Dysregulation / Disinhibition (-.51) (Gaughan et. al, 2009)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deliberation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Erratic life-style (-.57) (Gaughan et al., 2012); - Alcohol related problems (-.38) (Ruiz et al., 2010)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFI-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Soto &amp; John, 2016)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Conformity (-.36), - Tradition (-.24), + Stimulation (.21), + Positive affect  </t>
     </r>
     <r>
       <rPr>
@@ -854,7 +1140,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Gaughan et al., 2009</t>
+      <t xml:space="preserve">.32</t>
     </r>
     <r>
       <rPr>
@@ -867,23 +1153,27 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Compliance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tender-Mindedness</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Callous affect </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Power </t>
     </r>
     <r>
       <rPr>
@@ -904,7 +1194,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Gaughan, 2014; Gaughan et al., 2009</t>
+      <t xml:space="preserve">Soto &amp; John, 2016</t>
     </r>
     <r>
       <rPr>
@@ -919,33 +1209,18 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Competence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutifulness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Achievement Striving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Supervisor rating (Piedmont &amp; Weinstein, 1994)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Self-Discipline</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Attachment anxiety (Noftle &amp; Shaver, 2006); - Dysregulation / Disinhibition </t>
+    <t xml:space="preserve">Energy level</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Purpose in life (.53), + Self-acceptance (.53), + Social connectedness </t>
     </r>
     <r>
       <rPr>
@@ -966,7 +1241,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Gaughan et. al, 2009</t>
+      <t xml:space="preserve">.33</t>
     </r>
     <r>
       <rPr>
@@ -979,32 +1254,30 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Deliberation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Erratic life-style (Gaughan, 2014); - Alcohol related problems (Ruiz et al., 2010)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFI-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Conformity, - Tradition, + Stimulation, + Positive affect (Soto &amp; John, 2016)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Power </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Compassion</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Benevolence (.47), - Power (-.44), + Positive relations </t>
     </r>
     <r>
       <rPr>
@@ -1025,6 +1298,351 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">.41</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Respectfulness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Conformity </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.39</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Universalism (.21), + Likability </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.25</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Security </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.30</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Productiveness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hedonism (-.35), + Achievement (.26), + Environmental mastery (.56) (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Stimulation, + Autonomy (Soto &amp; John, 2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative Emotionality</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Autonomy </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-.32</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Positive relations (-.56), - Purpose in life (-.55), - Environmental mastery (-.65), -Self-acceptance(-.68), - Positive affect </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-.42</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Emotional Volatility</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Stress resistance </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">Soto &amp; John, 2016</t>
     </r>
     <r>
@@ -1040,30 +1658,21 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Energy level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Purpose in life, + Self-acceptance, + Social connectedness (Soto &amp; John, 2016)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compassion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Benevolence, - Power, + Positive relations (Soto &amp; John, 2016)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Respectfulness</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Conformity </t>
+    <t xml:space="preserve">Open-mindedness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intellectual curiosity</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Self-direction (.44), + Personal growth </t>
     </r>
     <r>
       <rPr>
@@ -1084,7 +1693,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Soto &amp; John, 2016</t>
+      <t xml:space="preserve">.50</t>
     </r>
     <r>
       <rPr>
@@ -1097,20 +1706,45 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Universalism, + Likability (Soto &amp; John, 2016)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Security </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Soto &amp; John, 2016)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Aesthetic Sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creative Imagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIP-NEO-120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Johnson, 2014)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inmoderation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Hangover symptoms </t>
     </r>
     <r>
       <rPr>
@@ -1131,7 +1765,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Soto &amp; John, 2016</t>
+      <t xml:space="preserve">.35</t>
     </r>
     <r>
       <rPr>
@@ -1144,32 +1778,33 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Productiveness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hedonism, + Achievement, + Environmental mastery (Soto &amp; John, 2016)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responsability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Stimulation, + Autonomy (Soto &amp; John, 2016)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Negative Emotionality</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Autonomy </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (McAdams &amp; Donnellan, 2009)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Friendliness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity Level</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Alcohol Use (.45), + Drinking problems </t>
     </r>
     <r>
       <rPr>
@@ -1190,7 +1825,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Soto &amp; John, 2016</t>
+      <t xml:space="preserve">.37</t>
     </r>
     <r>
       <rPr>
@@ -1203,23 +1838,30 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">- Positive relations, - Purpose in life, - Environmental mastery, -Self-acceptance, - Positive affect (Soto &amp; John, 2016)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emotional Volatility</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Stress resistance </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (McAdams &amp; Donnellan, 2009)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheerfulness</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Addictive mobile phone usage style </t>
     </r>
     <r>
       <rPr>
@@ -1240,7 +1882,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Soto &amp; John, 2016</t>
+      <t xml:space="preserve">.28</t>
     </r>
     <r>
       <rPr>
@@ -1253,38 +1895,45 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Open-mindedness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intellectual curiosity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Self-direction, + Personal growth (Soto &amp; John, 2016)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aesthetic Sensitivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creative Imagination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPIP-NEO-120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anger</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Academic achievement school </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Siddiqui, 2011)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Openness to Experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artistic interests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adventurousness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intellect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberalism</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Trendy mobile phone usage style </t>
     </r>
     <r>
       <rPr>
@@ -1305,7 +1954,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Rosander &amp; Bäckstörm, 2014</t>
+      <t xml:space="preserve">.31</t>
     </r>
     <r>
       <rPr>
@@ -1318,20 +1967,48 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Inmoderation</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Hangover symptoms </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Siddiqui, 2011)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Morality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Thrifty mobile phone usage style (.48) (Siddiqui, 2011)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooperation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sympathy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self-Efficacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orderliness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achievement-striving</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+ Academic Performance </t>
     </r>
     <r>
       <rPr>
@@ -1352,7 +2029,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">McAdams &amp; Donnellan, 2009</t>
+      <t xml:space="preserve">.23</t>
     </r>
     <r>
       <rPr>
@@ -1365,151 +2042,19 @@
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Friendliness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activity Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Alcohol Use, + Drinking problems (McAdams &amp; Donnellan, 2009)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheerfulness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Addictive mobile phone usage style (Siddiqui, 2011)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Openness to Experience</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imagination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artistic interests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adventurousness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intellect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liberalism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Trendy mobile phone usage style (Siddiqui, 2011)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Thrifty mobile phone usage style (Siddiqui, 2011)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooperation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sympathy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Self-Efficacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orderliness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Achievement-striving</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ Academic Performance </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rosander, Bäckström &amp; Sternberg, 2011</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">+ General health behaviors </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Hagger-Johnson &amp; Whiteman, 2007</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Rosander, Bäckström &amp; Sternberg, 2011)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">+ General health behaviors (.27) (Hagger-Johnson &amp; Whiteman, 2007)</t>
   </si>
   <si>
     <t xml:space="preserve">Cautiousness</t>
@@ -1522,7 +2067,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1558,6 +2103,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1616,7 +2174,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1653,6 +2211,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1680,8 +2242,8 @@
   </sheetPr>
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A111" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F126" activeCellId="0" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1690,7 +2252,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="70.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -1734,23 +2296,23 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,9 +2327,7 @@
       <c r="E5" s="4" t="n">
         <v>0.66</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,13 +2335,13 @@
       <c r="B6" s="4"/>
       <c r="C6" s="6"/>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>0.76</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -1789,16 +2349,16 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>0.81</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -1807,20 +2367,18 @@
       <c r="B8" s="4"/>
       <c r="C8" s="6"/>
       <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>0.68</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="F8" s="8"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1833,7 +2391,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>0.7</v>
@@ -1846,7 +2404,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>0.64</v>
@@ -1859,7 +2417,7 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>0.8</v>
@@ -1872,20 +2430,20 @@
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>0.7</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1898,12 +2456,14 @@
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>0.67</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,13 +2471,13 @@
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>0.76</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -1926,7 +2486,7 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>0.71</v>
@@ -1939,20 +2499,20 @@
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>0.76</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1965,7 +2525,7 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>0.74</v>
@@ -1978,7 +2538,7 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>0.66</v>
@@ -1991,7 +2551,7 @@
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>0.61</v>
@@ -2004,7 +2564,7 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>0.79</v>
@@ -2015,7 +2575,7 @@
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -2028,7 +2588,7 @@
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="4" t="n">
         <v>0.74</v>
@@ -2041,13 +2601,13 @@
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" s="4" t="n">
         <v>0.7</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="4"/>
     </row>
@@ -2056,13 +2616,13 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="4" t="n">
         <v>0.69</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -2071,43 +2631,41 @@
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>0.69</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="F29" s="5"/>
       <c r="G29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>0.66</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G30" s="4"/>
     </row>
@@ -2116,13 +2674,13 @@
       <c r="B31" s="4"/>
       <c r="C31" s="6"/>
       <c r="D31" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E31" s="4" t="n">
         <v>0.52</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G31" s="4"/>
     </row>
@@ -2130,10 +2688,10 @@
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E32" s="4" t="n">
         <v>0.75</v>
@@ -2148,12 +2706,14 @@
       <c r="B33" s="4"/>
       <c r="C33" s="6"/>
       <c r="D33" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E33" s="4" t="n">
         <v>0.66</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="G33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,11 +2727,13 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="5"/>
       <c r="G35" s="4" t="n">
@@ -2194,7 +2756,7 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E37" s="4" t="n">
         <v>0.78</v>
@@ -2280,7 +2842,7 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2377,7 +2939,7 @@
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -2470,7 +3032,7 @@
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -2488,7 +3050,9 @@
       <c r="E58" s="4" t="n">
         <v>0.79</v>
       </c>
-      <c r="F58" s="5"/>
+      <c r="F58" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="G58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,13 +3060,13 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E59" s="4" t="n">
         <v>0.71</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G59" s="4"/>
     </row>
@@ -2511,13 +3075,13 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E60" s="4" t="n">
         <v>0.75</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G60" s="4"/>
     </row>
@@ -2526,7 +3090,7 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E61" s="4" t="n">
         <v>0.59</v>
@@ -2539,7 +3103,7 @@
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E62" s="4" t="n">
         <v>0.67</v>
@@ -2552,20 +3116,20 @@
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E63" s="4" t="n">
         <v>0.56</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
       <c r="B64" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -2578,7 +3142,7 @@
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E65" s="4" t="n">
         <v>0.67</v>
@@ -2591,7 +3155,7 @@
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E66" s="4" t="n">
         <v>0.66</v>
@@ -2604,12 +3168,14 @@
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E67" s="4" t="n">
         <v>0.62</v>
       </c>
-      <c r="F67" s="5"/>
+      <c r="F67" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="G67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2617,13 +3183,13 @@
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E68" s="4" t="n">
         <v>0.67</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G68" s="4"/>
     </row>
@@ -2632,13 +3198,13 @@
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E69" s="4" t="n">
         <v>0.75</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G69" s="4"/>
     </row>
@@ -2647,13 +3213,13 @@
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E70" s="4" t="n">
         <v>0.71</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G70" s="4"/>
     </row>
@@ -2668,13 +3234,13 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="4" t="n">
@@ -2684,7 +3250,7 @@
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
       <c r="B73" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -2697,13 +3263,13 @@
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E74" s="4" t="n">
         <v>0.83</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G74" s="4"/>
     </row>
@@ -2718,7 +3284,7 @@
         <v>0.8</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G75" s="4"/>
     </row>
@@ -2727,20 +3293,20 @@
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E76" s="4" t="n">
         <v>0.74</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
       <c r="B77" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -2753,13 +3319,13 @@
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E78" s="4" t="n">
         <v>0.68</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G78" s="4"/>
     </row>
@@ -2768,13 +3334,13 @@
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E79" s="4" t="n">
         <v>0.66</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G79" s="4"/>
     </row>
@@ -2789,14 +3355,14 @@
         <v>0.75</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4"/>
       <c r="B81" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -2809,13 +3375,13 @@
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E82" s="4" t="n">
         <v>0.76</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G82" s="4"/>
     </row>
@@ -2824,13 +3390,13 @@
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E83" s="4" t="n">
         <v>0.74</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G83" s="4"/>
     </row>
@@ -2839,20 +3405,20 @@
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E84" s="4" t="n">
         <v>0.68</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4"/>
       <c r="B85" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -2865,13 +3431,13 @@
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E86" s="4" t="n">
         <v>0.79</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G86" s="4"/>
     </row>
@@ -2886,7 +3452,7 @@
         <v>0.74</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G87" s="4"/>
     </row>
@@ -2895,20 +3461,20 @@
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E88" s="4" t="n">
         <v>0.7</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4"/>
       <c r="B89" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -2921,13 +3487,13 @@
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E90" s="4" t="n">
         <v>0.78</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G90" s="4"/>
     </row>
@@ -2936,7 +3502,7 @@
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E91" s="4" t="n">
         <v>0.67</v>
@@ -2949,7 +3515,7 @@
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E92" s="4" t="n">
         <v>0.67</v>
@@ -2968,12 +3534,14 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="F94" s="5"/>
       <c r="G94" s="4" t="n">
         <v>120</v>
@@ -2995,7 +3563,7 @@
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E96" s="4" t="n">
         <v>0.78</v>
@@ -3008,7 +3576,7 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E97" s="4" t="n">
         <v>0.87</v>
@@ -3039,9 +3607,7 @@
       <c r="E99" s="4" t="n">
         <v>0.74</v>
       </c>
-      <c r="F99" s="5" t="s">
-        <v>131</v>
-      </c>
+      <c r="F99" s="5"/>
       <c r="G99" s="4"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,13 +3615,13 @@
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E100" s="4" t="n">
         <v>0.72</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G100" s="4"/>
     </row>
@@ -3075,7 +3641,7 @@
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -3088,7 +3654,7 @@
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E103" s="4" t="n">
         <v>0.81</v>
@@ -3127,7 +3693,7 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E106" s="4" t="n">
         <v>0.71</v>
@@ -3146,7 +3712,7 @@
         <v>0.77</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G107" s="4"/>
     </row>
@@ -3155,20 +3721,20 @@
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E108" s="4" t="n">
         <v>0.8</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G108" s="4"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -3181,7 +3747,7 @@
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E110" s="4" t="n">
         <v>0.83</v>
@@ -3194,7 +3760,7 @@
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E111" s="4" t="n">
         <v>0.76</v>
@@ -3207,7 +3773,7 @@
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E112" s="4" t="n">
         <v>0.69</v>
@@ -3220,7 +3786,7 @@
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E113" s="4" t="n">
         <v>0.72</v>
@@ -3233,7 +3799,7 @@
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E114" s="4" t="n">
         <v>0.75</v>
@@ -3246,20 +3812,20 @@
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E115" s="4" t="n">
         <v>0.64</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G115" s="4"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
@@ -3285,13 +3851,13 @@
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E118" s="4" t="n">
         <v>0.76</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G118" s="4"/>
     </row>
@@ -3300,7 +3866,7 @@
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E119" s="4" t="n">
         <v>0.76</v>
@@ -3313,7 +3879,7 @@
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E120" s="4" t="n">
         <v>0.73</v>
@@ -3326,7 +3892,7 @@
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E121" s="4" t="n">
         <v>0.76</v>
@@ -3339,7 +3905,7 @@
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E122" s="4" t="n">
         <v>0.72</v>
@@ -3350,7 +3916,7 @@
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4"/>
       <c r="B123" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
@@ -3363,7 +3929,7 @@
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E124" s="4" t="n">
         <v>0.63</v>
@@ -3376,7 +3942,7 @@
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E125" s="4" t="n">
         <v>0.83</v>
@@ -3389,7 +3955,7 @@
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E126" s="4" t="n">
         <v>0.69</v>
@@ -3402,13 +3968,13 @@
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E127" s="4" t="n">
         <v>0.8</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G127" s="4"/>
     </row>
@@ -3417,28 +3983,28 @@
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E128" s="4" t="n">
         <v>0.73</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G128" s="4"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="9"/>
-      <c r="B129" s="9"/>
-      <c r="C129" s="9"/>
-      <c r="D129" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E129" s="9" t="n">
+      <c r="A129" s="10"/>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E129" s="10" t="n">
         <v>0.87</v>
       </c>
-      <c r="F129" s="10"/>
-      <c r="G129" s="9"/>
+      <c r="F129" s="11"/>
+      <c r="G129" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>